<commit_message>
excel data sample, symbol and condition improve
</commit_message>
<xml_diff>
--- a/StockData.xlsx
+++ b/StockData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,22 +478,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NABIL</t>
+          <t>SHPC</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nabil Bank Limited</t>
+          <t>Sanima Mai Hydropower Ltd.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Commercial Banks</t>
+          <t>Hydro Power</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>270,569,970.00</t>
+          <t>30,892,510.00</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -501,11 +501,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>27,056,997,000.00</t>
+          <t>3,089,251,000.00</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>27.82</v>
+        <v>13.18</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -516,22 +516,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>KDL</t>
+          <t>NICA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kalinchowk Darshan Limited</t>
+          <t>NIC Asia Bank Ltd.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hotels And Tourism</t>
+          <t>Commercial Banks</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6,000,000.00</t>
+          <t>115,640,053.66</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -539,11 +539,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>600,000,000.00</t>
+          <t>11,564,005,366.00</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>5.32</v>
+        <v>40.22</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -554,22 +554,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NABIL</t>
+          <t>NTC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nabil Bank Limited</t>
+          <t>Nepal Doorsanchar Comapany Limited</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Commercial Banks</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>270,569,970.00</t>
+          <t>180,000,000.00</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -577,11 +577,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>27,056,997,000.00</t>
+          <t>18,000,000,000.00</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>27.82</v>
+        <v>43.36</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -592,22 +592,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KDL</t>
+          <t>SCB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kalinchowk Darshan Limited</t>
+          <t>Standard Chartered Bank Limited</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hotels And Tourism</t>
+          <t>Commercial Banks</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6,000,000.00</t>
+          <t>94,294,540.00</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -615,11 +615,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>600,000,000.00</t>
+          <t>9,429,454,000.00</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5.32</v>
+        <v>37.39</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -668,42 +668,954 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KDL</t>
+          <t>HBL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kalinchowk Darshan Limited</t>
+          <t>Himalayan Bank Limited</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hotels And Tourism</t>
+          <t>Commercial Banks</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6,000,000.00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+          <t>216,566,156.32</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>21,656,615,632.00</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>15.08</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>EIC</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Everest Insurance Co. Ltd.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Non-Life Insurance</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12,546,210.00</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1,254,621,000.00</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>(FY:078-079, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UPPER</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Upper Tamakoshi Hydropower Ltd</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hydro Power</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>105,900,000.00</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10,590,000,000.00</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>-35.49</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NIB</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Nepal Investment Bank Limited</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>190,398,426.40</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>19,039,842,640.00</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NBB</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Nepal Bangladesh Bank Limited</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>100,853,997.30</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>100</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>10,085,399,730.00</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>(FY:078-079, Q:3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Siddhartha Bank Limited</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>140,899,801.90</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>14,089,980,190.00</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>22.64</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PCBL</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Prime Commercial Bank Ltd.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>194,025,757.16</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>19,402,575,716.00</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>11.66</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sagarmatha Insurance Co. Ltd.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Non-Life Insurance</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>13,336,290.00</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>100</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>1,333,629,000.00</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SANIMA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sanima Bank Limited</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>124,601,150.59</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12,460,115,059.00</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>21.02</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MEGA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Mega Bank Nepal Ltd.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>167,652,799.08</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>16,765,279,908.00</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>GBIME</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Global IME Bank Limited</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>357,710,600.00</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>35,771,060,000.00</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>20.28</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CBBL</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Chhimek Laghubitta Bittiya Sanstha Limited</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Microfinance</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>28,354,020.00</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>100</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2,835,402,000.00</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>37.45</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>NIFRA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Nepal Infrastructure Bank Limited</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Investment</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>216,000,000.00</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>21,600,000,000.00</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PFL</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pokhara Finance Ltd.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10,825,566.10</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>100</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1,082,556,610.00</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>NIBPO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Nepal Investment Bank Ltd. Promoter Share</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Promotor Share</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>100</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>(FY:, Q:0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>EDBL</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Excel Development Bank Ltd.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Development Bank Limited</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>12,496,944.71</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>1,249,694,470.90</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>10.13</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>NLIC</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Nepal Life Insurance Co. Ltd.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Life Insurance</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>82,079,665.50</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>100</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>8,207,966,550.00</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>LICN</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Life Insurance Co. Nepal</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Life Insurance</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>26,532,000.00</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>100</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2,653,200,000.00</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>NHPC</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>National Hydro Power Company Limited</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Hydro Power</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>24,675,254.10</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>100</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2,467,525,410.00</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CIT</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Citizen Investment Trust</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Investment</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>53,137,500.00</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>100</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>5,313,750,000.00</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>17.08</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>JOSHI</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Joshi Hydropower Development Company Ltd</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Hydro Power</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3,714,000.00</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>371,400,000.00</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>(FY:077-078, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NMB Bank Limited</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Commercial Banks</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>183,667,060.00</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>100</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>18,366,706,000.00</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>18.57</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>HAMRO</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Hamro Bikas Bank Ltd.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Development Bank Limited</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5,040,533.70</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>100</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>504,053,370.00</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>(FY:075-076, Q:2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>API</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Api Power Company Ltd.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hydro Power</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>41,332,842.10</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>100</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>4,133,284,210.00</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>NRIC</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Nepal Re-Insurance Company Limited</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>122,033,750.00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>600,000,000.00</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5.32</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>(FY:079-080, Q:4)</t>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>12,203,375,000.00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>4.79</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>(FY:079-080, Q:2)</t>
         </is>
       </c>
     </row>

</xml_diff>